<commit_message>
Update copyright license date
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/DataTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/DataTest.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Quadratic" sheetId="1" r:id="rId1"/>
     <sheet name="LogNormal" sheetId="2" r:id="rId2"/>
-    <sheet name="rand" sheetId="3" r:id="rId3"/>
+    <sheet name="Prepend Bias" sheetId="4" r:id="rId3"/>
+    <sheet name="Insert SinX" sheetId="5" r:id="rId4"/>
+    <sheet name="rand" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>#0</t>
   </si>
@@ -1150,7 +1152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:D47"/>
     </sheetView>
   </sheetViews>
@@ -1857,10 +1859,342 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>201.80840065253633</v>
+      </c>
+      <c r="B3">
+        <v>58.620945862627487</v>
+      </c>
+      <c r="C3">
+        <v>220.07664709283972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>53.474705073569275</v>
+      </c>
+      <c r="B4">
+        <v>40.538545068143122</v>
+      </c>
+      <c r="C4">
+        <v>203.51751586612707</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>164.54951335302948</v>
+      </c>
+      <c r="B5">
+        <v>223.26358300929206</v>
+      </c>
+      <c r="C5">
+        <v>158.80600371765328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>184.43853081173009</v>
+      </c>
+      <c r="B6">
+        <v>39.376121216355287</v>
+      </c>
+      <c r="C6">
+        <v>176.20336574636445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>242.20012194299269</v>
+      </c>
+      <c r="B7">
+        <v>220.05464129806498</v>
+      </c>
+      <c r="C7">
+        <v>247.1748112585922</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f>A3</f>
+        <v>201.80840065253633</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="0">B3</f>
+        <v>58.620945862627487</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>220.07664709283972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:D12" si="1">A4</f>
+        <v>53.474705073569275</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>40.538545068143122</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>203.51751586612707</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:D13" si="2">A5</f>
+        <v>164.54951335302948</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>223.26358300929206</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>158.80600371765328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:D14" si="3">A6</f>
+        <v>184.43853081173009</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>39.376121216355287</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>176.20336574636445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:D15" si="4">A7</f>
+        <v>242.20012194299269</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="4"/>
+        <v>220.05464129806498</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="4"/>
+        <v>247.1748112585922</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>217.70577014018116</v>
+      </c>
+      <c r="B3">
+        <v>185.1832443345136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>212.10225356087059</v>
+      </c>
+      <c r="B4">
+        <v>123.65378860870956</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>242.90944645956762</v>
+      </c>
+      <c r="B5">
+        <v>50.186914376627733</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>163.10225874755912</v>
+      </c>
+      <c r="B6">
+        <v>209.60661879580667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>112.53261836089243</v>
+      </c>
+      <c r="B7">
+        <v>81.339067022672978</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A3</f>
+        <v>217.70577014018116</v>
+      </c>
+      <c r="B11">
+        <f>SIN(A11)</f>
+        <v>-0.80511957258355771</v>
+      </c>
+      <c r="C11">
+        <f>B3</f>
+        <v>185.1832443345136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" ref="A12:A15" si="0">A4</f>
+        <v>212.10225356087059</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:B15" si="1">SIN(A12)</f>
+        <v>-0.9989989107251156</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C15" si="2">B4</f>
+        <v>123.65378860870956</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>242.90944645956762</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>-0.8451320433706011</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>50.186914376627733</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>163.10225874755912</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>-0.25762095473463181</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>209.60661879580667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>112.53261836089243</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>-0.53517691820364299</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>81.339067022672978</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E20"/>
+      <selection activeCell="B6" sqref="B6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,901 +2202,901 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*255</f>
-        <v>41.217646766899321</v>
+        <v>242.08275577301305</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:G16" ca="1" si="0">RAND()*255</f>
-        <v>14.26004170284722</v>
+        <v>138.91224798653016</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>12.155398818730019</v>
+        <v>11.335223261822929</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>73.445078929566208</v>
+        <v>218.06139103902677</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>34.042554123396933</v>
+        <v>242.29307029402028</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>142.81377406708026</v>
+        <v>225.15115331389237</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3942457618446857</v>
+        <v>150.44739300178165</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:G30" ca="1" si="1">RAND()*255</f>
-        <v>2.5813722851669496</v>
+        <v>139.28310751429345</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>166.5138021375553</v>
+        <v>80.102572295671408</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>58.286706164473181</v>
+        <v>211.49916691409496</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>215.15262966391069</v>
+        <v>149.69592603922155</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>175.99545703871505</v>
+        <v>239.35528082772231</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>71.284704954872851</v>
+        <v>122.26832794754525</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>189.86531753650428</v>
+        <v>90.989072913668622</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>150.08390463066397</v>
+        <v>246.20085002037408</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>194.50824592923334</v>
+        <v>79.584061997130547</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>165.43999962240846</v>
+        <v>170.06684288745035</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>12.792089934455687</v>
+        <v>249.18255543585005</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>223.29888201241815</v>
+        <v>81.886104692959563</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>32.505521560388829</v>
+        <v>92.445521805846951</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>113.52091297963479</v>
+        <v>170.46921695288037</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>217.48873712468432</v>
+        <v>220.84688498666756</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>96.045719874676365</v>
+        <v>86.22895410578856</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>74.911099219747939</v>
+        <v>139.00351390828163</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>94.708826790226595</v>
+        <v>65.60549709247752</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>223.14254164809674</v>
+        <v>187.8252275164252</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>73.052548094544548</v>
+        <v>137.21800035694159</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>171.98848961904002</v>
+        <v>170.73346510907371</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>127.9196826577042</v>
+        <v>41.498017760383682</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>27.460407128464858</v>
+        <v>223.29081694147447</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>30.986108808597656</v>
+        <v>44.035977919076039</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>173.16359383492252</v>
+        <v>177.08776918052504</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>227.10717310582569</v>
+        <v>111.62390487037645</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>245.16352571142349</v>
+        <v>75.942543948372645</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>179.26481203333665</v>
+        <v>206.11856759082841</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>190.91146267642063</v>
+        <v>247.04762482176898</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>94.43549151857664</v>
+        <v>170.70354254800148</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>136.34445009202497</v>
+        <v>30.978988497606835</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>179.36455039298889</v>
+        <v>169.09860500361589</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>211.91953254188925</v>
+        <v>251.80845303501843</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>125.71204343853027</v>
+        <v>20.222865210828807</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>91.892890185917409</v>
+        <v>33.873565550951376</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>107.78019532212993</v>
+        <v>165.04639125963172</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>175.32097087590037</v>
+        <v>204.29212222319887</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>161.39038567457217</v>
+        <v>193.82711662066544</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>90.017416497751654</v>
+        <v>228.51861320653833</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>45.853675883539026</v>
+        <v>252.90490452167964</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>55.063483911269884</v>
+        <v>238.1716441550071</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>53.097845679166767</v>
+        <v>199.62141698977658</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>38.850533329292588</v>
+        <v>204.64743689195797</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4441087494168476</v>
+        <v>115.09423173663232</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>94.833950328370349</v>
+        <v>31.154198865612344</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>73.159614266989834</v>
+        <v>207.88127142626692</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>217.21951544206922</v>
+        <v>188.47614422571093</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>124.82025077693208</v>
+        <v>228.0623614509106</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9221478883480057</v>
+        <v>201.4582833786435</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>243.48305408566057</v>
+        <v>213.9479420080819</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>11.354476881556836</v>
+        <v>92.372105807578265</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>195.48123912720106</v>
+        <v>51.411863649304422</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>16.202419016232771</v>
+        <v>162.47349164633823</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>223.02883937814948</v>
+        <v>76.682077022820991</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>234.7921197006234</v>
+        <v>247.80006543103377</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>86.231076434740217</v>
+        <v>253.8428637648872</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>100.52090863103422</v>
+        <v>9.2261536823039858</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>252.78184002305795</v>
+        <v>83.613553765282674</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3795076981912864</v>
+        <v>42.29643525491683</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>220.18439374310259</v>
+        <v>110.63490205847754</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>196.30815408117275</v>
+        <v>114.17418421454579</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>239.21532019677679</v>
+        <v>240.29942442367752</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>33.355113718802954</v>
+        <v>157.16176960249982</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>247.57187761770135</v>
+        <v>165.10886783477574</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>159.80532676793047</v>
+        <v>206.47610974650507</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>63.293043735915582</v>
+        <v>96.611647228431607</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>129.2029795508351</v>
+        <v>7.5339126671120287</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>109.75491772035903</v>
+        <v>114.65156985666984</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>39.394679775526122</v>
+        <v>185.37953832174293</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>113.31782238628163</v>
+        <v>207.10832930052641</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>197.25652983422444</v>
+        <v>91.975403811707679</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>160.59618151962809</v>
+        <v>194.90288014836543</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>90.805579329244523</v>
+        <v>98.675759531258478</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>201.40842630777999</v>
+        <v>219.34462656376434</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>190.43684063471963</v>
+        <v>246.83329386505915</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>15.375092406687843</v>
+        <v>157.48151773464502</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>249.34732417766261</v>
+        <v>248.11469531147026</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4191735773088121</v>
+        <v>11.565147190448124</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>249.55934445684119</v>
+        <v>16.74300745059216</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>243.23142857165317</v>
+        <v>243.52295733339324</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>25.64477563885611</v>
+        <v>1.1801857180989894</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>211.19793317756253</v>
+        <v>27.495072500035789</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>204.65270147743644</v>
+        <v>54.309235251914778</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>45.765912168695614</v>
+        <v>128.84138717548294</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>182.54991708711083</v>
+        <v>204.42875695099897</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>140.16381373092668</v>
+        <v>48.929482415940022</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>204.99279062385986</v>
+        <v>6.6354401995157755</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>195.23043380291273</v>
+        <v>73.192000153863859</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>153.35463012909437</v>
+        <v>170.88505081947054</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>150.96650940836852</v>
+        <v>119.40561902188132</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>14.9623379504881</v>
+        <v>69.424598385290764</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>116.44286027523525</v>
+        <v>4.7336571525262974</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>73.358818010721905</v>
+        <v>231.54132776002319</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>229.03839488473548</v>
+        <v>202.63772071501299</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>179.77047240337032</v>
+        <v>254.37267063039823</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>159.90283299048536</v>
+        <v>144.52508730607406</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>165.26960153074495</v>
+        <v>153.5797578019706</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>218.38084327381864</v>
+        <v>85.461961442101966</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>75.71307601759645</v>
+        <v>133.73729884761332</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>194.67739066963253</v>
+        <v>42.682369039109005</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>216.23447787502604</v>
+        <v>91.20778662899329</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>77.935917169658921</v>
+        <v>165.17647877271961</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>240.72801628954693</v>
+        <v>162.1591265104606</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>68.584529333211577</v>
+        <v>236.63894979832389</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>67.2792173864636</v>
+        <v>246.62632219525494</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>192.30202671379769</v>
+        <v>198.62579631563963</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>189.50498393687502</v>
+        <v>34.205762176222478</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>15.492812551098035</v>
+        <v>65.423709306684245</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>20.411848346864531</v>
+        <v>216.4007764130719</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>221.76693137299034</v>
+        <v>202.92534082540629</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>202.02522541635733</v>
+        <v>217.60533578323543</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>128.70948037222041</v>
+        <v>234.89358316022651</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>61.333004193776688</v>
+        <v>120.62523227398354</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>239.9243418654307</v>
+        <v>166.09578004413706</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>16.90145451559129</v>
+        <v>59.520048520798667</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>13.455516858481595</v>
+        <v>29.39090515756428</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>27.61081430200732</v>
+        <v>120.12179586173195</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>137.88681945499576</v>
+        <v>217.48355389375587</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>62.71202384977979</v>
+        <v>85.299783840531802</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>149.38108791770628</v>
+        <v>253.51426248187471</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>76.89739723418883</v>
+        <v>107.11800669637356</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1554473765526581</v>
+        <v>136.35701892189155</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>46.903810437657391</v>
+        <v>74.318047770436351</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>171.78631599484802</v>
+        <v>22.535007643718021</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>27.859180894915475</v>
+        <v>175.59060091497423</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>187.59720569725175</v>
+        <v>61.344620381640922</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>135.16470996509375</v>
+        <v>69.669533960014476</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>126.39851344022564</v>
+        <v>140.16223068657663</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>244.92599688133726</v>
+        <v>16.986794261542546</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>28.914236643658842</v>
+        <v>51.108754669686377</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>177.38032797691153</v>
+        <v>161.60670014877351</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>84.949960876618931</v>
+        <v>13.037218593218837</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>56.466235457144293</v>
+        <v>192.71018736479547</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>208.88545066371043</v>
+        <v>1.7828064728476685</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>108.89642333273038</v>
+        <v>126.13206775079237</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>60.051684716297316</v>
+        <v>199.05357124796856</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>92.375307747726765</v>
+        <v>60.219608490469135</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>79.431843121636703</v>
+        <v>43.252189688994527</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>196.32195159639855</v>
+        <v>215.4320831369414</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>115.25926358072519</v>
+        <v>110.59984374327303</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>247.05451449446849</v>
+        <v>109.1566767637963</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>17.940216185600711</v>
+        <v>199.39791668868597</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6219949840016952</v>
+        <v>171.12869525414888</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>81.005761033727595</v>
+        <v>93.550565914730427</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>64.57995653137958</v>
+        <v>157.62519466494561</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>233.67138760388829</v>
+        <v>172.34431996466182</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>91.688669459834827</v>
+        <v>159.1109432292634</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>25.545737528243432</v>
+        <v>33.537551688940589</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>61.010384974722101</v>
+        <v>234.12841967624311</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>100.8016936845323</v>
+        <v>23.746647159762144</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>194.96248026963639</v>
+        <v>100.58606817802975</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>165.43235677083828</v>
+        <v>142.14585430241019</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>10.726261845485846</v>
+        <v>46.335700935743255</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>83.016647540499832</v>
+        <v>7.1346230373213615</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>116.62045369095975</v>
+        <v>155.07147601204593</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>154.44995261596816</v>
+        <v>235.77516626949748</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>173.30886791686632</v>
+        <v>27.33759584785378</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>116.63405767819177</v>
+        <v>116.38699962852806</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>201.57580775735087</v>
+        <v>2.7715855367359006</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>209.65310107167249</v>
+        <v>100.23331775599652</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>14.053191713620196</v>
+        <v>90.802075947384793</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>41.806297853463292</v>
+        <v>36.442443415749899</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>26.900672190410187</v>
+        <v>103.84637566092869</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>153.0988510150209</v>
+        <v>119.44715039055829</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>14.176525651619478</v>
+        <v>72.233654241190294</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>139.4063993184798</v>
+        <v>60.618392167316962</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>226.0469403625776</v>
+        <v>236.30634023196191</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>16.3430012706417</v>
+        <v>48.207381611321679</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>19.370611956627464</v>
+        <v>205.75277751531877</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>27.065636749179042</v>
+        <v>217.56880461372424</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>93.91852730964888</v>
+        <v>222.23075699342252</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>184.52564947235055</v>
+        <v>113.23167797222978</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3678574442837963</v>
+        <v>42.426284168751685</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>57.164902044017992</v>
+        <v>243.63982557428253</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>96.560772926893705</v>
+        <v>40.1380480574758</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>134.42843017874046</v>
+        <v>199.78687426478996</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>216.38854647403056</v>
+        <v>215.03271758921821</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>92.986412006058657</v>
+        <v>235.58438125262245</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>24.279535148689394</v>
+        <v>133.26680823069708</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>96.950972530752296</v>
+        <v>248.52149459891388</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>249.68953764395926</v>
+        <v>123.23512063410881</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>146.57469123351422</v>
+        <v>140.30071120246581</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>181.74301309481314</v>
+        <v>43.525956773418727</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>78.927481018104757</v>
+        <v>146.62130561790542</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>142.40947840495838</v>
+        <v>50.997895038146325</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>184.84181111900045</v>
+        <v>3.6328148762585517</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>194.85810739379895</v>
+        <v>32.128110154719153</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>21.449387024818176</v>
+        <v>83.09906215052429</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>242.91287847395017</v>
+        <v>85.687218848198086</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>29.587144973035176</v>
+        <v>163.10346793103398</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>84.31618266207667</v>
+        <v>111.87706443558586</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>29.801479839935173</v>
+        <v>197.0135285242616</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>230.41116900872223</v>
+        <v>227.11652035269725</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>45.874029064884652</v>
+        <v>27.927782453850696</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>236.10173594571924</v>
+        <v>157.18896097509884</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>183.50778044781234</v>
+        <v>150.56259723765413</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>150.12645637651781</v>
+        <v>116.00952400670293</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>31.459382106171425</v>
+        <v>123.2587855697454</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>209.56396305900444</v>
+        <v>62.302945942389613</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>113.67086272655862</v>
+        <v>2.7307456687293916</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>26.587111377328608</v>
+        <v>33.000445813307678</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>231.85607218099952</v>
+        <v>187.2032506208794</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>201.89975176288399</v>
+        <v>134.26248358062546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>